<commit_message>
Ask remove hub data
</commit_message>
<xml_diff>
--- a/lang/lang.xlsx
+++ b/lang/lang.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="507">
   <si>
     <t xml:space="preserve">part</t>
   </si>
@@ -1472,6 +1472,78 @@
   </si>
   <si>
     <t xml:space="preserve">HUB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confirm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remove_hub_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Möchten Sie die HUB-Daten auch entfernen? Falls Sie später einmal auf HUB2 wechseln möchten, können die Daten übernommen werden. Allenfalls möchten Sie das HUB-Plugin nur deaktivieren?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to remove the HUB data as well? If you want to switch to HUB2 later, the data can be transferred. At most, you just want to disable the HUB plugin?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cancel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remove</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hub_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entferne HUB-Daten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove HUB data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUB-Daten behalten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep HUB data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUB-Plugin nur deaktivieren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Just deactivate HUB plugin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUB-Daten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUB data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">removed_hub_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die HUB-Daten wurden auch entfernt!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The HUB data was also removed!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kept_hub_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die HUB-Daten wurden behalten!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The HUB data was kept!</t>
   </si>
 </sst>
 </file>
@@ -1593,10 +1665,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E254"/>
+  <dimension ref="A1:E262"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A254" activeCellId="0" sqref="A254"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A238" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A263" activeCellId="0" sqref="A263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5162,6 +5234,115 @@
         <v>482</v>
       </c>
     </row>
+    <row r="255" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D255" s="1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B256" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D256" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="D257" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="D258" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="D259" s="1" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="D260" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="C261" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="D261" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="D262" s="1" t="s">
+        <v>506</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Rename uninstall language keys
</commit_message>
<xml_diff>
--- a/lang/lang.xlsx
+++ b/lang/lang.xlsx
@@ -1474,61 +1474,97 @@
     <t xml:space="preserve">HUB</t>
   </si>
   <si>
-    <t xml:space="preserve">confirm</t>
+    <t xml:space="preserve">uninstall</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">confirm_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">remove_hub_data</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Möchten Sie die Hub-Daten auch entfernen? Falls Sie später einmal auf Hub2 wechseln möchten, können die Daten übernommen werden. Allenfalls möchten Sie das Hub-Plugin nur deaktivieren?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you want to remove the Hub data as well? If you want to switch to Hub2 later, the data can be transferred. At most, you just want to disable the Hub plugin?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cancel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancel</t>
   </si>
   <si>
     <t xml:space="preserve">remove_hub_data</t>
   </si>
   <si>
-    <t xml:space="preserve">Möchten Sie die Hub-Daten auch entfernen? Falls Sie später einmal auf Hub2 wechseln möchten, können die Daten übernommen werden. Allenfalls möchten Sie das Hub-Plugin nur deaktivieren?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do you want to remove the Hub data as well? If you want to switch to Hub2 later, the data can be transferred. At most, you just want to disable the Hub plugin?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cancel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cancel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">remove</t>
+    <t xml:space="preserve">Entferne Hub-Daten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove Hub data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keep_hub_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hub-Daten behalten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep Hub data</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">deactivate_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">hub</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Hub-Plugin nur deaktivieren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Just deactivate Hub plugin</t>
   </si>
   <si>
     <t xml:space="preserve">hub_data</t>
   </si>
   <si>
-    <t xml:space="preserve">Entferne Hub-Daten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remove Hub data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">keep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hub-Daten behalten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keep Hub data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hub-Plugin nur deaktivieren</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Just deactivate Hub plugin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hub-Daten</t>
   </si>
   <si>
     <t xml:space="preserve">Hub data</t>
   </si>
   <si>
-    <t xml:space="preserve">removed_hub_data</t>
+    <t xml:space="preserve">msg_removed_hub_data</t>
   </si>
   <si>
     <t xml:space="preserve">Die Hub-Daten wurden auch entfernt!</t>
@@ -1537,7 +1573,7 @@
     <t xml:space="preserve">The Hub data was also removed!</t>
   </si>
   <si>
-    <t xml:space="preserve">kept_hub_data</t>
+    <t xml:space="preserve">msg_kept_hub_data</t>
   </si>
   <si>
     <t xml:space="preserve">Die Hub-Daten wurden behalten!</t>
@@ -1553,7 +1589,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1583,6 +1619,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1627,7 +1669,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1646,6 +1688,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1668,7 +1714,7 @@
   <dimension ref="A1:E262"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A241" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B262" activeCellId="0" sqref="B262"/>
+      <selection pane="topLeft" activeCell="A255" activeCellId="0" sqref="A255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5238,7 +5284,7 @@
       <c r="A255" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="B255" s="1" t="s">
+      <c r="B255" s="5" t="s">
         <v>484</v>
       </c>
       <c r="C255" s="1" t="s">
@@ -5259,40 +5305,40 @@
         <v>488</v>
       </c>
     </row>
-    <row r="257" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B257" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="B257" s="1" t="s">
+      <c r="C257" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="C257" s="1" t="s">
+      <c r="D257" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="D257" s="1" t="s">
+    </row>
+    <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B258" s="1" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="258" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A258" s="1" t="s">
+      <c r="C258" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="B258" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="C258" s="1" t="s">
+      <c r="D258" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="D258" s="1" t="s">
+    </row>
+    <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B259" s="5" t="s">
         <v>495</v>
-      </c>
-    </row>
-    <row r="259" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B259" s="1" t="s">
-        <v>215</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>496</v>
@@ -5301,9 +5347,9 @@
         <v>497</v>
       </c>
     </row>
-    <row r="260" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="1" t="s">
-        <v>215</v>
+        <v>483</v>
       </c>
       <c r="B260" s="1" t="s">
         <v>498</v>
@@ -5315,9 +5361,9 @@
         <v>500</v>
       </c>
     </row>
-    <row r="261" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="1" t="s">
-        <v>268</v>
+        <v>483</v>
       </c>
       <c r="B261" s="1" t="s">
         <v>501</v>
@@ -5329,9 +5375,9 @@
         <v>503</v>
       </c>
     </row>
-    <row r="262" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="1" t="s">
-        <v>268</v>
+        <v>483</v>
       </c>
       <c r="B262" s="1" t="s">
         <v>504</v>

</xml_diff>